<commit_message>
Add experiment script generation
</commit_message>
<xml_diff>
--- a/experiments/hyperparams.xlsx
+++ b/experiments/hyperparams.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\RHWSL\home\rmontanana\Code\benchmark\experiments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rmontanana/Code/benchmark/experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D43B55-AE13-4F8B-95ED-B4E1421D9B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD878A8-3447-A643-BDE2-54CD84B6EA41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4414" yWindow="1431" windowWidth="22697" windowHeight="14469" activeTab="1" xr2:uid="{911CFC2C-8BEE-48A1-A861-96D551AF7A0B}"/>
+    <workbookView xWindow="4420" yWindow="1440" windowWidth="22700" windowHeight="14460" activeTab="1" xr2:uid="{911CFC2C-8BEE-48A1-A861-96D551AF7A0B}"/>
   </bookViews>
   <sheets>
     <sheet name="STree" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
   <si>
     <t>C</t>
   </si>
@@ -97,13 +97,19 @@
     <t>max_samples</t>
   </si>
   <si>
-    <t>"auto"</t>
-  </si>
-  <si>
     <t>"impurity"</t>
   </si>
   <si>
     <t>"rbf"</t>
+  </si>
+  <si>
+    <t>"sqrt"</t>
+  </si>
+  <si>
+    <t>"best"</t>
+  </si>
+  <si>
+    <t>0.75</t>
   </si>
 </sst>
 </file>
@@ -344,9 +350,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -354,61 +357,64 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -730,111 +736,111 @@
       <selection activeCell="B11" sqref="B11:M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.52734375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="13.17578125" customWidth="1"/>
-    <col min="7" max="7" width="13.3515625" customWidth="1"/>
-    <col min="8" max="8" width="14.1171875" customWidth="1"/>
-    <col min="9" max="9" width="14.52734375" customWidth="1"/>
-    <col min="11" max="11" width="16.1171875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5859375" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="10.8203125" style="4"/>
+    <col min="1" max="1" width="5.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="11" max="11" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="B2" s="11" t="s">
+    <row r="1" spans="1:16" s="3" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="13"/>
-    </row>
-    <row r="3" spans="1:16" s="1" customFormat="1" ht="104.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="5"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="10" t="s">
+      <c r="M2" s="11"/>
+    </row>
+    <row r="3" spans="1:16" s="1" customFormat="1" ht="104.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="10"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="B4" s="16"/>
-      <c r="C4" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="9">
+      <c r="L3" s="8"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B4" s="14"/>
+      <c r="C4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="7">
         <v>10000</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8">
+      <c r="E4" s="6"/>
+      <c r="F4" s="6">
         <v>4</v>
       </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8">
+      <c r="G4" s="6"/>
+      <c r="H4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6">
         <v>24</v>
       </c>
-      <c r="M4" s="17"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="B5" s="18" t="str">
+      <c r="M4" s="15"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B5" s="16" t="str">
         <f>IF(B4&lt;&gt;"",CONCATENATE(CHAR(34),B2,CHAR(34),": ",B4,", "),"")</f>
         <v/>
       </c>
@@ -878,10 +884,10 @@
         <f t="shared" ref="L5" si="7">IF(L4&lt;&gt;"",CONCATENATE(CHAR(34),L2,CHAR(34),": ",L4,", "),"")</f>
         <v xml:space="preserve">"max_features": 24, </v>
       </c>
-      <c r="M5" s="19"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="B6" s="18" t="str">
+      <c r="M5" s="17"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B6" s="16" t="str">
         <f>IF(B4&lt;&gt;"",CONCATENATE(CHAR(34),"base_estimator__",B2,CHAR(34),": ",B4,", "),"")</f>
         <v/>
       </c>
@@ -925,125 +931,125 @@
         <f t="shared" si="8"/>
         <v xml:space="preserve">"base_estimator__max_features": 24, </v>
       </c>
-      <c r="M6" s="19" t="str">
+      <c r="M6" s="17" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="B7" s="20" t="str">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B7" s="24" t="str">
         <f>IF(I4&lt;&gt;"",CONCATENATE(CHAR(34),I2,CHAR(34),": ",I4,", "),"")</f>
         <v/>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="21"/>
-    </row>
-    <row r="8" spans="1:16" ht="14.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="6"/>
-      <c r="B8" s="22" t="str">
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="26"/>
+    </row>
+    <row r="8" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="18" t="str">
         <f>_xlfn.CONCAT("'{",LEFT(_xlfn.CONCAT(B5:L5),LEN(_xlfn.CONCAT(B5:L5))-2),"}'")</f>
         <v>'{"kernel": "rbf", "max_iter": 10000, "degree": 4, "split_criteria": "impurity", "max_features": 24}'</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="23"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="A9" s="6"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="23"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="B10" s="20"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="21"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="B11" s="22" t="str">
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="20"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="20"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B10" s="24"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="26"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B11" s="18" t="str">
         <f>_xlfn.CONCAT("'{",LEFT(_xlfn.CONCAT(B6:L6),LEN(_xlfn.CONCAT(B6:L6))-2),"}'")</f>
         <v>'{"base_estimator__kernel": "rbf", "base_estimator__max_iter": 10000, "base_estimator__degree": 4, "base_estimator__split_criteria": "impurity", "base_estimator__max_features": 24}'</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="23"/>
-    </row>
-    <row r="12" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="24"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="26"/>
-    </row>
-    <row r="13" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="14" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="15" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="16" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="17" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="18" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="19" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="20" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="21" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="22" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="23" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="24" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="25" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="26" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="27" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="28" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="29" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="30" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="31" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="20"/>
+    </row>
+    <row r="12" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="21"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="23"/>
+    </row>
+    <row r="13" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="17" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="18" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="19" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="20" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="21" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="22" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B8:M9"/>
@@ -1060,96 +1066,100 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2045EF00-4ABD-464E-B35B-A864DABCBA74}">
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:M19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21:M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.52734375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="13.17578125" customWidth="1"/>
-    <col min="3" max="3" width="11.87890625" customWidth="1"/>
-    <col min="4" max="4" width="11.5859375" customWidth="1"/>
-    <col min="5" max="5" width="12.05859375" customWidth="1"/>
-    <col min="7" max="7" width="13.3515625" customWidth="1"/>
-    <col min="8" max="8" width="14.1171875" customWidth="1"/>
-    <col min="9" max="9" width="14.52734375" customWidth="1"/>
-    <col min="11" max="11" width="16.1171875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5859375" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="10.8203125" style="4"/>
+    <col min="1" max="1" width="5.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="11" max="11" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="2" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="11" t="s">
+    <row r="1" spans="1:16" s="3" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="13"/>
-    </row>
-    <row r="3" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="14"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="15"/>
-    </row>
-    <row r="4" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="B4" s="16">
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="11"/>
+    </row>
+    <row r="3" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="12"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="13"/>
+    </row>
+    <row r="4" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="14">
         <v>10</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="6">
         <v>100</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="17"/>
-    </row>
-    <row r="5" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="B5" s="18" t="str">
+      <c r="D4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="15"/>
+    </row>
+    <row r="5" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="16" t="str">
         <f>IF(B4&lt;&gt;"",CONCATENATE(CHAR(34),B2,CHAR(34),": ",B4,", "),"")</f>
         <v xml:space="preserve">"n_jobs": 10, </v>
       </c>
       <c r="C5" s="2" t="str">
-        <f t="shared" ref="C5:L5" si="0">IF(C4&lt;&gt;"",CONCATENATE(CHAR(34),C2,CHAR(34),": ",C4,", "),"")</f>
+        <f t="shared" ref="C5:E5" si="0">IF(C4&lt;&gt;"",CONCATENATE(CHAR(34),C2,CHAR(34),": ",C4,", "),"")</f>
         <v xml:space="preserve">"n_estimators": 100, </v>
       </c>
       <c r="D5" s="2" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v xml:space="preserve">"max_features": "sqrt", </v>
       </c>
       <c r="E5" s="2" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v xml:space="preserve">"max_samples": 0.75, </v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -1158,24 +1168,24 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
-      <c r="M5" s="19"/>
-    </row>
-    <row r="6" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="18" t="str">
+      <c r="M5" s="17"/>
+    </row>
+    <row r="6" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="16" t="str">
         <f>IF(B4&lt;&gt;"",CONCATENATE(CHAR(34),"base_estimator__",B2,CHAR(34),": ",B4,", "),"")</f>
         <v xml:space="preserve">"base_estimator__n_jobs": 10, </v>
       </c>
       <c r="C6" s="2" t="str">
-        <f t="shared" ref="C6:M6" si="1">IF(C4&lt;&gt;"",CONCATENATE(CHAR(34),"base_estimator__",C2,CHAR(34),": ",C4,", "),"")</f>
+        <f t="shared" ref="C6:E6" si="1">IF(C4&lt;&gt;"",CONCATENATE(CHAR(34),"base_estimator__",C2,CHAR(34),": ",C4,", "),"")</f>
         <v xml:space="preserve">"base_estimator__n_estimators": 100, </v>
       </c>
       <c r="D6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v xml:space="preserve">"base_estimator__max_features": "sqrt", </v>
       </c>
       <c r="E6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v xml:space="preserve">"base_estimator__max_samples": 0.75, </v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -1184,165 +1194,161 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
-      <c r="M6" s="19"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="B7" s="20" t="str">
+      <c r="M6" s="17"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B7" s="24" t="str">
         <f>IF(I4&lt;&gt;"",CONCATENATE(CHAR(34),I2,CHAR(34),": ",I4,", "),"")</f>
         <v/>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="21"/>
-    </row>
-    <row r="8" spans="1:16" ht="14.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="6"/>
-      <c r="B8" s="22" t="str">
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="26"/>
+    </row>
+    <row r="8" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="18" t="str">
         <f>_xlfn.CONCAT("'{",LEFT(_xlfn.CONCAT(B5:L5),LEN(_xlfn.CONCAT(B5:L5))-2),"}'")</f>
-        <v>'{"n_jobs": 10, "n_estimators": 100}'</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="23"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="A9" s="6"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="23"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="B10" s="20"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="21"/>
-    </row>
-    <row r="11" spans="1:16" s="4" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="B12" s="11" t="s">
+        <v>'{"n_jobs": 10, "n_estimators": 100, "max_features": "sqrt", "max_samples": 0.75}'</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="20"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="20"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B10" s="24"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="26"/>
+    </row>
+    <row r="11" spans="1:16" s="3" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B12" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="G12" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="H12" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="12" t="s">
+      <c r="I12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="12" t="s">
+      <c r="J12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="12" t="s">
+      <c r="K12" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="L12" s="12" t="s">
+      <c r="L12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="M12" s="13"/>
-    </row>
-    <row r="13" spans="1:16" s="1" customFormat="1" ht="104.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="5"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="10" t="s">
+      <c r="M12" s="11"/>
+    </row>
+    <row r="13" spans="1:16" s="1" customFormat="1" ht="104.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10" t="s">
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I13" s="10" t="s">
+      <c r="I13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J13" s="10" t="s">
+      <c r="J13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="K13" s="10" t="s">
+      <c r="K13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="L13" s="10"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="B14" s="16"/>
-      <c r="C14" s="8" t="s">
+      <c r="L13" s="8"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B14" s="14"/>
+      <c r="C14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="9">
-        <v>10000</v>
-      </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8">
-        <v>4</v>
-      </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M14" s="17"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="B15" s="18" t="str">
+      <c r="M14" s="15"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B15" s="16" t="str">
         <f>IF(B14&lt;&gt;"",CONCATENATE(CHAR(34),B12,CHAR(34),": ",B14,", "),"")</f>
         <v/>
       </c>
@@ -1352,7 +1358,7 @@
       </c>
       <c r="D15" s="2" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"max_iter": 10000, </v>
+        <v/>
       </c>
       <c r="E15" s="2" t="str">
         <f t="shared" si="2"/>
@@ -1360,7 +1366,7 @@
       </c>
       <c r="F15" s="2" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"degree": 4, </v>
+        <v/>
       </c>
       <c r="G15" s="2" t="str">
         <f t="shared" si="2"/>
@@ -1368,7 +1374,7 @@
       </c>
       <c r="H15" s="2" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"split_criteria": "impurity", </v>
+        <v/>
       </c>
       <c r="I15" s="2" t="str">
         <f t="shared" si="2"/>
@@ -1376,7 +1382,7 @@
       </c>
       <c r="J15" s="2" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v xml:space="preserve">"splitter": "best", </v>
       </c>
       <c r="K15" s="2" t="str">
         <f t="shared" si="2"/>
@@ -1384,12 +1390,12 @@
       </c>
       <c r="L15" s="2" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"max_features": "auto", </v>
-      </c>
-      <c r="M15" s="19"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="B16" s="18" t="str">
+        <v xml:space="preserve">"max_features": "sqrt", </v>
+      </c>
+      <c r="M15" s="17"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B16" s="16" t="str">
         <f>IF(B14&lt;&gt;"",CONCATENATE(CHAR(34),"base_estimator__",B12,CHAR(34),": ",B14,", "),"")</f>
         <v/>
       </c>
@@ -1399,7 +1405,7 @@
       </c>
       <c r="D16" s="2" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">"base_estimator__max_iter": 10000, </v>
+        <v/>
       </c>
       <c r="E16" s="2" t="str">
         <f t="shared" si="3"/>
@@ -1407,7 +1413,7 @@
       </c>
       <c r="F16" s="2" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">"base_estimator__degree": 4, </v>
+        <v/>
       </c>
       <c r="G16" s="2" t="str">
         <f t="shared" si="3"/>
@@ -1415,7 +1421,7 @@
       </c>
       <c r="H16" s="2" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">"base_estimator__split_criteria": "impurity", </v>
+        <v/>
       </c>
       <c r="I16" s="2" t="str">
         <f t="shared" si="3"/>
@@ -1423,7 +1429,7 @@
       </c>
       <c r="J16" s="2" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v xml:space="preserve">"base_estimator__splitter": "best", </v>
       </c>
       <c r="K16" s="2" t="str">
         <f t="shared" si="3"/>
@@ -1431,127 +1437,127 @@
       </c>
       <c r="L16" s="2" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">"base_estimator__max_features": "auto", </v>
-      </c>
-      <c r="M16" s="19" t="str">
+        <v xml:space="preserve">"base_estimator__max_features": "sqrt", </v>
+      </c>
+      <c r="M16" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="B17" s="20" t="str">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B17" s="24" t="str">
         <f>IF(I14&lt;&gt;"",CONCATENATE(CHAR(34),I12,CHAR(34),": ",I14,", "),"")</f>
         <v/>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="21"/>
-    </row>
-    <row r="18" spans="1:13" ht="14.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="6"/>
-      <c r="B18" s="22" t="str">
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="26"/>
+    </row>
+    <row r="18" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5"/>
+      <c r="B18" s="18" t="str">
         <f>_xlfn.CONCAT(LEFT(_xlfn.CONCAT(B15:L15),LEN(_xlfn.CONCAT(B15:L15))-2))</f>
-        <v>"kernel": "rbf", "max_iter": 10000, "degree": 4, "split_criteria": "impurity", "max_features": "auto"</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="23"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A19" s="6"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="23"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="B20" s="20"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="21"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="B21" s="22" t="str">
+        <v>"kernel": "rbf", "splitter": "best", "max_features": "sqrt"</v>
+      </c>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="20"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="5"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="20"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B20" s="24"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="25"/>
+      <c r="M20" s="26"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B21" s="18" t="str">
         <f>_xlfn.CONCAT(LEFT(B8,LEN(B8)-2),", ",CHAR(34),"be_hyperparams",CHAR(34),":  ",CHAR(34),"{",SUBSTITUTE(_xlfn.CONCAT(B18:L18),CHAR(34),CONCATENATE("\",CHAR(34))),"}",CHAR(34),"}'")</f>
-        <v>'{"n_jobs": 10, "n_estimators": 100, "be_hyperparams":  "{\"kernel\": \"rbf\", \"max_iter\": 10000, \"degree\": 4, \"split_criteria\": \"impurity\", \"max_features\": \"auto\"}"}'</v>
-      </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="23"/>
-    </row>
-    <row r="22" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B22" s="24"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
-      <c r="M22" s="26"/>
-    </row>
-    <row r="23" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="24" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="25" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="26" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="27" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="28" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="29" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="30" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="31" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="32" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="33" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="34" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="35" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="36" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="37" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="38" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="39" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="40" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="41" s="4" customFormat="1" x14ac:dyDescent="0.5"/>
+        <v>'{"n_jobs": 10, "n_estimators": 100, "max_features": "sqrt", "max_samples": 0.75, "be_hyperparams":  "{\"kernel\": \"rbf\", \"splitter\": \"best\", \"max_features\": \"sqrt\"}"}'</v>
+      </c>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="20"/>
+    </row>
+    <row r="22" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="21"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="23"/>
+    </row>
+    <row r="23" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="B17:M17"/>

</xml_diff>

<commit_message>
Prepare pseudo random forest experiments
</commit_message>
<xml_diff>
--- a/experiments/hyperparams.xlsx
+++ b/experiments/hyperparams.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rmontanana/Code/benchmark/experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD878A8-3447-A643-BDE2-54CD84B6EA41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B3EF40-192D-F64F-A0E0-1259E9B2773E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4420" yWindow="1440" windowWidth="22700" windowHeight="14460" activeTab="1" xr2:uid="{911CFC2C-8BEE-48A1-A861-96D551AF7A0B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
   <si>
     <t>C</t>
   </si>
@@ -110,6 +110,12 @@
   </si>
   <si>
     <t>0.75</t>
+  </si>
+  <si>
+    <t>"ovr"</t>
+  </si>
+  <si>
+    <t>"liblinear"</t>
   </si>
 </sst>
 </file>
@@ -1066,8 +1072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2045EF00-4ABD-464E-B35B-A864DABCBA74}">
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:M22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1330,7 +1336,7 @@
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B14" s="14"/>
       <c r="C14" s="6" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="6"/>
@@ -1341,10 +1347,10 @@
       <c r="J14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6" t="s">
-        <v>22</v>
-      </c>
+      <c r="K14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L14" s="6"/>
       <c r="M14" s="15"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
@@ -1354,7 +1360,7 @@
       </c>
       <c r="C15" s="2" t="str">
         <f t="shared" ref="C15:L15" si="2">IF(C14&lt;&gt;"",CONCATENATE(CHAR(34),C12,CHAR(34),": ",C14,", "),"")</f>
-        <v xml:space="preserve">"kernel": "rbf", </v>
+        <v xml:space="preserve">"kernel": "liblinear", </v>
       </c>
       <c r="D15" s="2" t="str">
         <f t="shared" si="2"/>
@@ -1386,11 +1392,11 @@
       </c>
       <c r="K15" s="2" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v xml:space="preserve">"multiclass_strategy": "ovr", </v>
       </c>
       <c r="L15" s="2" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"max_features": "sqrt", </v>
+        <v/>
       </c>
       <c r="M15" s="17"/>
     </row>
@@ -1401,7 +1407,7 @@
       </c>
       <c r="C16" s="2" t="str">
         <f t="shared" ref="C16:M16" si="3">IF(C14&lt;&gt;"",CONCATENATE(CHAR(34),"base_estimator__",C12,CHAR(34),": ",C14,", "),"")</f>
-        <v xml:space="preserve">"base_estimator__kernel": "rbf", </v>
+        <v xml:space="preserve">"base_estimator__kernel": "liblinear", </v>
       </c>
       <c r="D16" s="2" t="str">
         <f t="shared" si="3"/>
@@ -1433,11 +1439,11 @@
       </c>
       <c r="K16" s="2" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v xml:space="preserve">"base_estimator__multiclass_strategy": "ovr", </v>
       </c>
       <c r="L16" s="2" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">"base_estimator__max_features": "sqrt", </v>
+        <v/>
       </c>
       <c r="M16" s="17" t="str">
         <f t="shared" si="3"/>
@@ -1465,7 +1471,7 @@
       <c r="A18" s="5"/>
       <c r="B18" s="18" t="str">
         <f>_xlfn.CONCAT(LEFT(_xlfn.CONCAT(B15:L15),LEN(_xlfn.CONCAT(B15:L15))-2))</f>
-        <v>"kernel": "rbf", "splitter": "best", "max_features": "sqrt"</v>
+        <v>"kernel": "liblinear", "splitter": "best", "multiclass_strategy": "ovr"</v>
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
@@ -1511,7 +1517,7 @@
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B21" s="18" t="str">
         <f>_xlfn.CONCAT(LEFT(B8,LEN(B8)-2),", ",CHAR(34),"be_hyperparams",CHAR(34),":  ",CHAR(34),"{",SUBSTITUTE(_xlfn.CONCAT(B18:L18),CHAR(34),CONCATENATE("\",CHAR(34))),"}",CHAR(34),"}'")</f>
-        <v>'{"n_jobs": 10, "n_estimators": 100, "max_features": "sqrt", "max_samples": 0.75, "be_hyperparams":  "{\"kernel\": \"rbf\", \"splitter\": \"best\", \"max_features\": \"sqrt\"}"}'</v>
+        <v>'{"n_jobs": 10, "n_estimators": 100, "max_features": "sqrt", "max_samples": 0.75, "be_hyperparams":  "{\"kernel\": \"liblinear\", \"splitter\": \"best\", \"multiclass_strategy\": \"ovr\"}"}'</v>
       </c>
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>

</xml_diff>